<commit_message>
update Duty domain and services
</commit_message>
<xml_diff>
--- a/src/main/resources/DutyList.xlsx
+++ b/src/main/resources/DutyList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cagrigurbuz\Desktop\dutyassignment\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5697588-1694-4E08-9CDB-AFE568BEEDAC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A31E3DE7-C38F-494B-A21B-79E1785E8DB6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="21">
   <si>
     <t>Region</t>
   </si>
@@ -68,9 +68,6 @@
     <t>2020-02-15</t>
   </si>
   <si>
-    <t>taskCount</t>
-  </si>
-  <si>
     <t>deneme2</t>
   </si>
   <si>
@@ -87,13 +84,28 @@
   </si>
   <si>
     <t>02:00</t>
+  </si>
+  <si>
+    <t>dutyLoad</t>
+  </si>
+  <si>
+    <t>dutyType</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>SA</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -113,6 +125,15 @@
       <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="162"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -136,7 +157,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -153,7 +174,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -436,7 +463,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -448,10 +475,10 @@
     <col min="4" max="4" width="9.42578125" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.42578125" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.140625" style="2"/>
-    <col min="7" max="7" width="15" style="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15" style="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
@@ -470,16 +497,19 @@
       <c r="F1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="6" t="s">
-        <v>10</v>
+      <c r="G1" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>9</v>
@@ -493,16 +523,19 @@
       <c r="F2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="6">
+      <c r="G2" s="8">
+        <v>10.23</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+      <c r="B3" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>12</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>9</v>
@@ -516,31 +549,37 @@
       <c r="F3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G3" s="6">
-        <v>10</v>
+      <c r="G3" s="8">
+        <v>20.5</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="E4" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="F4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G4" s="6">
-        <v>10</v>
+      <c r="G4" s="8">
+        <v>12.6</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update duty domain importer and template
</commit_message>
<xml_diff>
--- a/src/main/resources/DutyList.xlsx
+++ b/src/main/resources/DutyList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cagrigurbuz\Desktop\dutyassignment\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A31E3DE7-C38F-494B-A21B-79E1785E8DB6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AB4A517-F50E-4E12-A42C-4F31D3B83307}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$F$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!#REF!</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,85 +36,50 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Region</t>
   </si>
   <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>startTime</t>
-  </si>
-  <si>
-    <t>endTime</t>
-  </si>
-  <si>
-    <t>startDate</t>
-  </si>
-  <si>
-    <t>endDate</t>
-  </si>
-  <si>
-    <t>deneme1</t>
-  </si>
-  <si>
-    <t>10:00</t>
-  </si>
-  <si>
-    <t>14:00</t>
-  </si>
-  <si>
-    <t>2020-02-15</t>
-  </si>
-  <si>
-    <t>deneme2</t>
-  </si>
-  <si>
-    <t>deneme</t>
-  </si>
-  <si>
-    <t>2020-02-16</t>
-  </si>
-  <si>
-    <t>08:00</t>
-  </si>
-  <si>
-    <t>deneme3</t>
-  </si>
-  <si>
-    <t>02:00</t>
-  </si>
-  <si>
     <t>dutyLoad</t>
   </si>
   <si>
     <t>dutyType</t>
   </si>
   <si>
-    <t>S</t>
-  </si>
-  <si>
-    <t>A</t>
-  </si>
-  <si>
-    <t>SA</t>
+    <t>employeeCode</t>
+  </si>
+  <si>
+    <t>employeeName</t>
+  </si>
+  <si>
+    <t>StartDate</t>
+  </si>
+  <si>
+    <t>StartTime</t>
+  </si>
+  <si>
+    <t>EndDate</t>
+  </si>
+  <si>
+    <t>EndTime</t>
+  </si>
+  <si>
+    <t>dutyDate</t>
+  </si>
+  <si>
+    <t>dutyName</t>
+  </si>
+  <si>
+    <t>employeePhone</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -157,32 +122,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -463,127 +412,67 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:M1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="2"/>
-    <col min="2" max="2" width="21.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" style="2"/>
-    <col min="7" max="7" width="15" style="8" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.140625" style="4"/>
+    <col min="9" max="9" width="9.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="3" t="s">
+      <c r="I1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="H1" s="6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>8</v>
-      </c>
-      <c r="G2" s="8">
-        <v>10.23</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G3" s="8">
-        <v>20.5</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G4" s="8">
-        <v>12.6</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>20</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Update domain importers accordingly
</commit_message>
<xml_diff>
--- a/src/main/resources/DutyList.xlsx
+++ b/src/main/resources/DutyList.xlsx
@@ -1,23 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23029"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cagrigurbuz\Desktop\dutyassignment\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AB4A517-F50E-4E12-A42C-4F31D3B83307}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89A1584E-EE1F-4FAD-8CAC-70E66445BB3A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{1880ADC9-5349-4884-BC50-6C9D5375E6F7}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="DutyList" sheetId="2" r:id="rId1"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!#REF!</definedName>
-  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -36,23 +33,32 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+  <si>
+    <t>Tarih</t>
+  </si>
+  <si>
+    <t>kod</t>
+  </si>
+  <si>
+    <t>sicilno</t>
+  </si>
+  <si>
+    <t>peradi</t>
+  </si>
+  <si>
+    <t>Telefon</t>
+  </si>
   <si>
     <t>Region</t>
   </si>
   <si>
+    <t>dutyType</t>
+  </si>
+  <si>
     <t>dutyLoad</t>
   </si>
   <si>
-    <t>dutyType</t>
-  </si>
-  <si>
-    <t>employeeCode</t>
-  </si>
-  <si>
-    <t>employeeName</t>
-  </si>
-  <si>
     <t>StartDate</t>
   </si>
   <si>
@@ -65,29 +71,20 @@
     <t>EndTime</t>
   </si>
   <si>
-    <t>dutyDate</t>
-  </si>
-  <si>
-    <t>dutyName</t>
-  </si>
-  <si>
-    <t>employeePhone</t>
+    <t>Priority</t>
+  </si>
+  <si>
+    <t>totalWorkingHour</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -122,16 +119,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -166,7 +159,7 @@
         <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent1>
       <a:accent2>
         <a:srgbClr val="ED7D31"/>
@@ -178,7 +171,7 @@
         <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent5>
       <a:accent6>
         <a:srgbClr val="70AD47"/>
@@ -225,6 +218,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -260,6 +270,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -411,68 +438,74 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CEE0D249-F716-4DDE-A9CB-1E2EE69DB74E}">
+  <dimension ref="A1:Z1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.140625" style="4"/>
-    <col min="9" max="9" width="9.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.42578125" style="4" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.140625" style="1"/>
+    <col min="1" max="1" width="10.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="6.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.140625" style="1"/>
+    <col min="9" max="9" width="10.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="7.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="17.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="26" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>8</v>
+      <c r="M1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>